<commit_message>
Tarea Gato y Caballos
</commit_message>
<xml_diff>
--- a/Tarea 01/a asterisco.xlsx
+++ b/Tarea 01/a asterisco.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUIS MARIO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUIS MARIO\Desktop\inteligencia-artificial\Tarea 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2E1BD79-5AC2-4B69-A109-2CC910A5D012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C210127B-8421-49B6-8D43-97A07D69200D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9EABACAB-6045-4FF3-A839-AA62EDF9777C}"/>
   </bookViews>
@@ -341,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -460,15 +460,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -506,6 +500,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -825,7 +837,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.453125" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -841,34 +853,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40">
+      <c r="A1" s="54">
         <v>1</v>
       </c>
-      <c r="B1" s="41">
+      <c r="B1" s="55">
         <v>160</v>
       </c>
-      <c r="C1" s="48">
+      <c r="C1" s="46">
         <v>2</v>
       </c>
-      <c r="D1" s="41">
-        <v>160</v>
-      </c>
-      <c r="E1" s="48">
+      <c r="D1" s="40">
+        <v>154</v>
+      </c>
+      <c r="E1" s="46">
         <v>3</v>
       </c>
-      <c r="F1" s="41">
-        <v>160</v>
-      </c>
-      <c r="G1" s="48">
+      <c r="F1" s="40">
+        <v>154</v>
+      </c>
+      <c r="G1" s="46">
         <v>4</v>
       </c>
-      <c r="H1" s="49">
-        <v>160</v>
-      </c>
-      <c r="I1" s="48">
+      <c r="H1" s="47">
+        <v>154</v>
+      </c>
+      <c r="I1" s="58">
         <v>5</v>
       </c>
-      <c r="J1" s="41">
+      <c r="J1" s="55">
         <v>160</v>
       </c>
       <c r="K1" s="1">
@@ -883,34 +895,34 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42">
+      <c r="A2" s="56">
         <v>50</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="57">
         <v>110</v>
       </c>
-      <c r="C2" s="50">
-        <v>60</v>
-      </c>
-      <c r="D2" s="43">
+      <c r="C2" s="48">
+        <v>54</v>
+      </c>
+      <c r="D2" s="41">
         <v>100</v>
       </c>
-      <c r="E2" s="50">
-        <v>70</v>
-      </c>
-      <c r="F2" s="43">
+      <c r="E2" s="48">
+        <v>64</v>
+      </c>
+      <c r="F2" s="41">
         <v>90</v>
       </c>
-      <c r="G2" s="50">
+      <c r="G2" s="48">
+        <v>74</v>
+      </c>
+      <c r="H2" s="49">
         <v>80</v>
       </c>
-      <c r="H2" s="51">
-        <v>80</v>
-      </c>
-      <c r="I2" s="50">
+      <c r="I2" s="59">
         <v>90</v>
       </c>
-      <c r="J2" s="43">
+      <c r="J2" s="57">
         <v>70</v>
       </c>
       <c r="K2" s="4">
@@ -923,10 +935,10 @@
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44">
+      <c r="A3" s="42">
         <v>8</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="43">
         <v>140</v>
       </c>
       <c r="C3" s="9">
@@ -941,11 +953,11 @@
         <v>11</v>
       </c>
       <c r="H3" s="10"/>
-      <c r="I3" s="52">
+      <c r="I3" s="50">
         <v>12</v>
       </c>
-      <c r="J3" s="45">
-        <v>154</v>
+      <c r="J3" s="43">
+        <v>148</v>
       </c>
       <c r="K3" s="11">
         <v>13</v>
@@ -959,10 +971,10 @@
       <c r="N3" s="12"/>
     </row>
     <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46">
+      <c r="A4" s="44">
         <v>40</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="45">
         <v>100</v>
       </c>
       <c r="C4" s="14"/>
@@ -971,10 +983,10 @@
       <c r="F4" s="15"/>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="53">
-        <v>94</v>
-      </c>
-      <c r="J4" s="47">
+      <c r="I4" s="51">
+        <v>88</v>
+      </c>
+      <c r="J4" s="45">
         <v>60</v>
       </c>
       <c r="K4" s="6">
@@ -987,10 +999,10 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44">
+      <c r="A5" s="42">
         <v>15</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="43">
         <v>120</v>
       </c>
       <c r="C5" s="11">
@@ -1007,11 +1019,11 @@
         <v>18</v>
       </c>
       <c r="H5" s="10"/>
-      <c r="I5" s="52">
+      <c r="I5" s="50">
         <v>19</v>
       </c>
-      <c r="J5" s="45">
-        <v>154</v>
+      <c r="J5" s="43">
+        <v>148</v>
       </c>
       <c r="K5" s="9">
         <v>20</v>
@@ -1025,10 +1037,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46">
+      <c r="A6" s="44">
         <v>30</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="45">
         <v>90</v>
       </c>
       <c r="C6" s="6">
@@ -1041,10 +1053,10 @@
       <c r="F6" s="13"/>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="53">
-        <v>104</v>
-      </c>
-      <c r="J6" s="47">
+      <c r="I6" s="51">
+        <v>98</v>
+      </c>
+      <c r="J6" s="45">
         <v>50</v>
       </c>
       <c r="K6" s="14"/>
@@ -1057,10 +1069,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="44">
+      <c r="A7" s="42">
         <v>22</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="43">
         <v>100</v>
       </c>
       <c r="C7" s="11">
@@ -1077,17 +1089,17 @@
         <v>25</v>
       </c>
       <c r="H7" s="10"/>
-      <c r="I7" s="52">
+      <c r="I7" s="22">
         <v>26</v>
       </c>
-      <c r="J7" s="45">
+      <c r="J7" s="23">
         <v>154</v>
       </c>
-      <c r="K7" s="52">
+      <c r="K7" s="50">
         <v>27</v>
       </c>
-      <c r="L7" s="45">
-        <v>148</v>
+      <c r="L7" s="43">
+        <v>142</v>
       </c>
       <c r="M7" s="11">
         <v>28</v>
@@ -1097,10 +1109,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46">
+      <c r="A8" s="44">
         <v>20</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="45">
         <v>80</v>
       </c>
       <c r="C8" s="6">
@@ -1113,16 +1125,16 @@
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="53">
+      <c r="I8" s="34">
         <v>114</v>
       </c>
-      <c r="J8" s="47">
+      <c r="J8" s="35">
         <v>40</v>
       </c>
-      <c r="K8" s="50">
-        <v>118</v>
-      </c>
-      <c r="L8" s="43">
+      <c r="K8" s="48">
+        <v>112</v>
+      </c>
+      <c r="L8" s="41">
         <v>30</v>
       </c>
       <c r="M8" s="4">
@@ -1133,10 +1145,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="44">
+      <c r="A9" s="42">
         <v>29</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="43">
         <v>80</v>
       </c>
       <c r="C9" s="22">
@@ -1161,18 +1173,18 @@
         <v>34</v>
       </c>
       <c r="L9" s="10"/>
-      <c r="M9" s="52">
+      <c r="M9" s="50">
         <v>35</v>
       </c>
-      <c r="N9" s="54">
-        <v>142</v>
+      <c r="N9" s="52">
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="46">
+      <c r="A10" s="44">
         <v>10</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="45">
         <v>70</v>
       </c>
       <c r="C10" s="34">
@@ -1189,10 +1201,10 @@
       <c r="J10" s="19"/>
       <c r="K10" s="14"/>
       <c r="L10" s="15"/>
-      <c r="M10" s="53">
-        <v>132</v>
-      </c>
-      <c r="N10" s="55">
+      <c r="M10" s="51">
+        <v>126</v>
+      </c>
+      <c r="N10" s="53">
         <v>10</v>
       </c>
     </row>
@@ -1234,7 +1246,9 @@
       <c r="M11" s="24">
         <v>41</v>
       </c>
-      <c r="N11" s="25"/>
+      <c r="N11" s="25">
+        <v>136</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="26">
@@ -1269,8 +1283,12 @@
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="31"/>
+      <c r="M12" s="30">
+        <v>136</v>
+      </c>
+      <c r="N12" s="31">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>